<commit_message>
Work on #403 - added a second worksheet to the Excel file used in PHPUnit tests.
</commit_message>
<xml_diff>
--- a/tests/assets/excel/sample_metadata.xlsx
+++ b/tests/assets/excel/sample_metadata.xlsx
@@ -5,17 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="126">
   <si>
     <t>ID</t>
   </si>
@@ -390,6 +391,9 @@
   </si>
   <si>
     <t>postcard_20.jpg</t>
+  </si>
+  <si>
+    <t>Some other worksheet.</t>
   </si>
 </sst>
 </file>
@@ -404,6 +408,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -487,7 +492,7 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1003,4 +1008,36 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>